<commit_message>
more test runs with simpler rule
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="log" localSheetId="0">Tabelle1!$A$1:$H$196</definedName>
+    <definedName name="log" localSheetId="0">Tabelle1!$A$1:$H$233</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="15">
   <si>
     <t>lra</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>zuendorf</t>
+  </si>
+  <si>
+    <t>input_models/TTC_InputRDG_Small1.xmi</t>
   </si>
 </sst>
 </file>
@@ -423,22 +426,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H196"/>
+  <dimension ref="A1:H233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -5535,6 +5538,968 @@
       </c>
       <c r="H196" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>42506.756712962961</v>
+      </c>
+      <c r="B197" t="s">
+        <v>13</v>
+      </c>
+      <c r="C197">
+        <v>286817</v>
+      </c>
+      <c r="D197">
+        <v>-22.855555555555501</v>
+      </c>
+      <c r="E197">
+        <v>100</v>
+      </c>
+      <c r="F197" t="s">
+        <v>6</v>
+      </c>
+      <c r="G197">
+        <v>301</v>
+      </c>
+      <c r="H197" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>42510.721400462964</v>
+      </c>
+      <c r="B198" t="s">
+        <v>13</v>
+      </c>
+      <c r="C198">
+        <v>8989</v>
+      </c>
+      <c r="D198">
+        <v>4</v>
+      </c>
+      <c r="E198">
+        <v>100</v>
+      </c>
+      <c r="F198" t="s">
+        <v>1</v>
+      </c>
+      <c r="G198">
+        <v>5</v>
+      </c>
+      <c r="H198" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>42510.72146990741</v>
+      </c>
+      <c r="B199" t="s">
+        <v>13</v>
+      </c>
+      <c r="C199">
+        <v>6368</v>
+      </c>
+      <c r="D199">
+        <v>4</v>
+      </c>
+      <c r="E199">
+        <v>100</v>
+      </c>
+      <c r="F199" t="s">
+        <v>4</v>
+      </c>
+      <c r="G199">
+        <v>5</v>
+      </c>
+      <c r="H199" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>42510.72148148148</v>
+      </c>
+      <c r="B200" t="s">
+        <v>13</v>
+      </c>
+      <c r="C200">
+        <v>731</v>
+      </c>
+      <c r="D200">
+        <v>4</v>
+      </c>
+      <c r="E200">
+        <v>100</v>
+      </c>
+      <c r="F200" t="s">
+        <v>5</v>
+      </c>
+      <c r="G200">
+        <v>5</v>
+      </c>
+      <c r="H200" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>42510.721574074072</v>
+      </c>
+      <c r="B201" t="s">
+        <v>13</v>
+      </c>
+      <c r="C201">
+        <v>8076</v>
+      </c>
+      <c r="D201">
+        <v>4</v>
+      </c>
+      <c r="E201">
+        <v>100</v>
+      </c>
+      <c r="F201" t="s">
+        <v>6</v>
+      </c>
+      <c r="G201">
+        <v>5</v>
+      </c>
+      <c r="H201" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>42510.721608796295</v>
+      </c>
+      <c r="B202" t="s">
+        <v>13</v>
+      </c>
+      <c r="C202">
+        <v>3377</v>
+      </c>
+      <c r="D202">
+        <v>2.5833333333333299</v>
+      </c>
+      <c r="E202">
+        <v>100</v>
+      </c>
+      <c r="F202" t="s">
+        <v>1</v>
+      </c>
+      <c r="G202">
+        <v>11</v>
+      </c>
+      <c r="H202" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>42510.721678240741</v>
+      </c>
+      <c r="B203" t="s">
+        <v>13</v>
+      </c>
+      <c r="C203">
+        <v>5415</v>
+      </c>
+      <c r="D203">
+        <v>1.49999999999999</v>
+      </c>
+      <c r="E203">
+        <v>100</v>
+      </c>
+      <c r="F203" t="s">
+        <v>4</v>
+      </c>
+      <c r="G203">
+        <v>9</v>
+      </c>
+      <c r="H203" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>42510.721724537034</v>
+      </c>
+      <c r="B204" t="s">
+        <v>13</v>
+      </c>
+      <c r="C204">
+        <v>4329</v>
+      </c>
+      <c r="D204">
+        <v>2.5833333333333299</v>
+      </c>
+      <c r="E204">
+        <v>100</v>
+      </c>
+      <c r="F204" t="s">
+        <v>5</v>
+      </c>
+      <c r="G204">
+        <v>11</v>
+      </c>
+      <c r="H204" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>42510.72184027778</v>
+      </c>
+      <c r="B205" t="s">
+        <v>13</v>
+      </c>
+      <c r="C205">
+        <v>10208</v>
+      </c>
+      <c r="D205">
+        <v>2.2166666666666601</v>
+      </c>
+      <c r="E205">
+        <v>100</v>
+      </c>
+      <c r="F205" t="s">
+        <v>6</v>
+      </c>
+      <c r="G205">
+        <v>9</v>
+      </c>
+      <c r="H205" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>42510.721886574072</v>
+      </c>
+      <c r="B206" t="s">
+        <v>13</v>
+      </c>
+      <c r="C206">
+        <v>4357</v>
+      </c>
+      <c r="D206">
+        <v>-7</v>
+      </c>
+      <c r="E206">
+        <v>100</v>
+      </c>
+      <c r="F206" t="s">
+        <v>1</v>
+      </c>
+      <c r="G206">
+        <v>31</v>
+      </c>
+      <c r="H206" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>42510.721944444442</v>
+      </c>
+      <c r="B207" t="s">
+        <v>13</v>
+      </c>
+      <c r="C207">
+        <v>4373</v>
+      </c>
+      <c r="D207">
+        <v>3</v>
+      </c>
+      <c r="E207">
+        <v>100</v>
+      </c>
+      <c r="F207" t="s">
+        <v>4</v>
+      </c>
+      <c r="G207">
+        <v>24</v>
+      </c>
+      <c r="H207" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>42510.722291666665</v>
+      </c>
+      <c r="B208" t="s">
+        <v>13</v>
+      </c>
+      <c r="C208">
+        <v>30384</v>
+      </c>
+      <c r="D208">
+        <v>5.0357142857142803</v>
+      </c>
+      <c r="E208">
+        <v>100</v>
+      </c>
+      <c r="F208" t="s">
+        <v>5</v>
+      </c>
+      <c r="G208">
+        <v>18</v>
+      </c>
+      <c r="H208" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>42510.722546296296</v>
+      </c>
+      <c r="B209" t="s">
+        <v>13</v>
+      </c>
+      <c r="C209">
+        <v>21913</v>
+      </c>
+      <c r="D209">
+        <v>5.0357142857142803</v>
+      </c>
+      <c r="E209">
+        <v>100</v>
+      </c>
+      <c r="F209" t="s">
+        <v>6</v>
+      </c>
+      <c r="G209">
+        <v>18</v>
+      </c>
+      <c r="H209" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>42510.722708333335</v>
+      </c>
+      <c r="B210" t="s">
+        <v>13</v>
+      </c>
+      <c r="C210">
+        <v>14131</v>
+      </c>
+      <c r="D210">
+        <v>-36</v>
+      </c>
+      <c r="E210">
+        <v>100</v>
+      </c>
+      <c r="F210" t="s">
+        <v>1</v>
+      </c>
+      <c r="G210">
+        <v>78</v>
+      </c>
+      <c r="H210" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>42510.72283564815</v>
+      </c>
+      <c r="B211" t="s">
+        <v>13</v>
+      </c>
+      <c r="C211">
+        <v>11043</v>
+      </c>
+      <c r="D211">
+        <v>-16.630952380952301</v>
+      </c>
+      <c r="E211">
+        <v>100</v>
+      </c>
+      <c r="F211" t="s">
+        <v>4</v>
+      </c>
+      <c r="G211">
+        <v>65</v>
+      </c>
+      <c r="H211" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>42510.723032407404</v>
+      </c>
+      <c r="B212" t="s">
+        <v>13</v>
+      </c>
+      <c r="C212">
+        <v>16308</v>
+      </c>
+      <c r="D212">
+        <v>-34</v>
+      </c>
+      <c r="E212">
+        <v>100</v>
+      </c>
+      <c r="F212" t="s">
+        <v>5</v>
+      </c>
+      <c r="G212">
+        <v>77</v>
+      </c>
+      <c r="H212" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>42510.723483796297</v>
+      </c>
+      <c r="B213" t="s">
+        <v>13</v>
+      </c>
+      <c r="C213">
+        <v>39263</v>
+      </c>
+      <c r="D213">
+        <v>9.0309433364988898</v>
+      </c>
+      <c r="E213">
+        <v>100</v>
+      </c>
+      <c r="F213" t="s">
+        <v>6</v>
+      </c>
+      <c r="G213">
+        <v>33</v>
+      </c>
+      <c r="H213" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>42510.723946759259</v>
+      </c>
+      <c r="B214" t="s">
+        <v>13</v>
+      </c>
+      <c r="C214">
+        <v>39619</v>
+      </c>
+      <c r="D214">
+        <v>-78</v>
+      </c>
+      <c r="E214">
+        <v>100</v>
+      </c>
+      <c r="F214" t="s">
+        <v>1</v>
+      </c>
+      <c r="G214">
+        <v>159</v>
+      </c>
+      <c r="H214" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>42510.724259259259</v>
+      </c>
+      <c r="B215" t="s">
+        <v>13</v>
+      </c>
+      <c r="C215">
+        <v>27647</v>
+      </c>
+      <c r="D215">
+        <v>-57.6666666666666</v>
+      </c>
+      <c r="E215">
+        <v>100</v>
+      </c>
+      <c r="F215" t="s">
+        <v>4</v>
+      </c>
+      <c r="G215">
+        <v>147</v>
+      </c>
+      <c r="H215" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>42511.891956018517</v>
+      </c>
+      <c r="B216" t="s">
+        <v>13</v>
+      </c>
+      <c r="C216">
+        <v>100757719</v>
+      </c>
+      <c r="D216">
+        <v>1.5</v>
+      </c>
+      <c r="E216">
+        <v>50</v>
+      </c>
+      <c r="F216" t="s">
+        <v>4</v>
+      </c>
+      <c r="G216">
+        <v>1</v>
+      </c>
+      <c r="H216" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>42513.554537037038</v>
+      </c>
+      <c r="B217" t="s">
+        <v>13</v>
+      </c>
+      <c r="C217">
+        <v>4583</v>
+      </c>
+      <c r="D217">
+        <v>4</v>
+      </c>
+      <c r="E217">
+        <v>50</v>
+      </c>
+      <c r="F217" t="s">
+        <v>4</v>
+      </c>
+      <c r="G217">
+        <v>5</v>
+      </c>
+      <c r="H217" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>42513.554745370369</v>
+      </c>
+      <c r="B218" t="s">
+        <v>13</v>
+      </c>
+      <c r="C218">
+        <v>5308</v>
+      </c>
+      <c r="D218">
+        <v>4</v>
+      </c>
+      <c r="E218">
+        <v>50</v>
+      </c>
+      <c r="F218" t="s">
+        <v>4</v>
+      </c>
+      <c r="G218">
+        <v>5</v>
+      </c>
+      <c r="H218" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>42513.575844907406</v>
+      </c>
+      <c r="B219" t="s">
+        <v>13</v>
+      </c>
+      <c r="C219">
+        <v>1731090</v>
+      </c>
+      <c r="D219">
+        <v>4</v>
+      </c>
+      <c r="E219">
+        <v>50</v>
+      </c>
+      <c r="F219" t="s">
+        <v>4</v>
+      </c>
+      <c r="G219">
+        <v>5</v>
+      </c>
+      <c r="H219" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>42513.576863425929</v>
+      </c>
+      <c r="B220" t="s">
+        <v>13</v>
+      </c>
+      <c r="C220">
+        <v>3910</v>
+      </c>
+      <c r="D220">
+        <v>4</v>
+      </c>
+      <c r="E220">
+        <v>50</v>
+      </c>
+      <c r="F220" t="s">
+        <v>4</v>
+      </c>
+      <c r="G220">
+        <v>5</v>
+      </c>
+      <c r="H220" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>42513.61822916667</v>
+      </c>
+      <c r="B221" t="s">
+        <v>13</v>
+      </c>
+      <c r="C221">
+        <v>3552</v>
+      </c>
+      <c r="D221">
+        <v>3</v>
+      </c>
+      <c r="E221">
+        <v>50</v>
+      </c>
+      <c r="F221" t="s">
+        <v>4</v>
+      </c>
+      <c r="G221">
+        <v>4</v>
+      </c>
+      <c r="H221" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>42513.622824074075</v>
+      </c>
+      <c r="B222" t="s">
+        <v>13</v>
+      </c>
+      <c r="C222">
+        <v>384751</v>
+      </c>
+      <c r="D222">
+        <v>3</v>
+      </c>
+      <c r="E222">
+        <v>50</v>
+      </c>
+      <c r="F222" t="s">
+        <v>4</v>
+      </c>
+      <c r="G222">
+        <v>4</v>
+      </c>
+      <c r="H222" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>42513.62363425926</v>
+      </c>
+      <c r="B223" t="s">
+        <v>13</v>
+      </c>
+      <c r="C223">
+        <v>2859</v>
+      </c>
+      <c r="D223">
+        <v>1.55</v>
+      </c>
+      <c r="E223">
+        <v>50</v>
+      </c>
+      <c r="F223" t="s">
+        <v>4</v>
+      </c>
+      <c r="G223">
+        <v>4</v>
+      </c>
+      <c r="H223" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>42513.624120370368</v>
+      </c>
+      <c r="B224" t="s">
+        <v>13</v>
+      </c>
+      <c r="C224">
+        <v>25715</v>
+      </c>
+      <c r="D224">
+        <v>1.9083333333333301</v>
+      </c>
+      <c r="E224">
+        <v>500</v>
+      </c>
+      <c r="F224" t="s">
+        <v>4</v>
+      </c>
+      <c r="G224">
+        <v>6</v>
+      </c>
+      <c r="H224" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>42513.624456018515</v>
+      </c>
+      <c r="B225" t="s">
+        <v>13</v>
+      </c>
+      <c r="C225">
+        <v>3355</v>
+      </c>
+      <c r="D225">
+        <v>3</v>
+      </c>
+      <c r="E225">
+        <v>100</v>
+      </c>
+      <c r="F225" t="s">
+        <v>1</v>
+      </c>
+      <c r="G225">
+        <v>4</v>
+      </c>
+      <c r="H225" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>42513.624502314815</v>
+      </c>
+      <c r="B226" t="s">
+        <v>13</v>
+      </c>
+      <c r="C226">
+        <v>4375</v>
+      </c>
+      <c r="D226">
+        <v>3</v>
+      </c>
+      <c r="E226">
+        <v>100</v>
+      </c>
+      <c r="F226" t="s">
+        <v>4</v>
+      </c>
+      <c r="G226">
+        <v>4</v>
+      </c>
+      <c r="H226" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>42513.624513888892</v>
+      </c>
+      <c r="B227" t="s">
+        <v>13</v>
+      </c>
+      <c r="C227">
+        <v>1116</v>
+      </c>
+      <c r="D227">
+        <v>3</v>
+      </c>
+      <c r="E227">
+        <v>100</v>
+      </c>
+      <c r="F227" t="s">
+        <v>5</v>
+      </c>
+      <c r="G227">
+        <v>4</v>
+      </c>
+      <c r="H227" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>42513.625740740739</v>
+      </c>
+      <c r="B228" t="s">
+        <v>13</v>
+      </c>
+      <c r="C228">
+        <v>97911</v>
+      </c>
+      <c r="D228">
+        <v>3</v>
+      </c>
+      <c r="E228">
+        <v>2000</v>
+      </c>
+      <c r="F228" t="s">
+        <v>4</v>
+      </c>
+      <c r="G228">
+        <v>8</v>
+      </c>
+      <c r="H228" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>42513.627962962964</v>
+      </c>
+      <c r="B229" t="s">
+        <v>13</v>
+      </c>
+      <c r="C229">
+        <v>7175</v>
+      </c>
+      <c r="D229">
+        <v>3</v>
+      </c>
+      <c r="E229">
+        <v>100</v>
+      </c>
+      <c r="F229" t="s">
+        <v>1</v>
+      </c>
+      <c r="G229">
+        <v>4</v>
+      </c>
+      <c r="H229" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>42513.628009259257</v>
+      </c>
+      <c r="B230" t="s">
+        <v>13</v>
+      </c>
+      <c r="C230">
+        <v>4611</v>
+      </c>
+      <c r="D230">
+        <v>3</v>
+      </c>
+      <c r="E230">
+        <v>100</v>
+      </c>
+      <c r="F230" t="s">
+        <v>4</v>
+      </c>
+      <c r="G230">
+        <v>4</v>
+      </c>
+      <c r="H230" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>42513.628020833334</v>
+      </c>
+      <c r="B231" t="s">
+        <v>13</v>
+      </c>
+      <c r="C231">
+        <v>1133</v>
+      </c>
+      <c r="D231">
+        <v>3</v>
+      </c>
+      <c r="E231">
+        <v>100</v>
+      </c>
+      <c r="F231" t="s">
+        <v>5</v>
+      </c>
+      <c r="G231">
+        <v>4</v>
+      </c>
+      <c r="H231" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>42513.631597222222</v>
+      </c>
+      <c r="B232" t="s">
+        <v>13</v>
+      </c>
+      <c r="C232">
+        <v>302556</v>
+      </c>
+      <c r="D232">
+        <v>3</v>
+      </c>
+      <c r="E232">
+        <v>5000</v>
+      </c>
+      <c r="F232" t="s">
+        <v>4</v>
+      </c>
+      <c r="G232">
+        <v>8</v>
+      </c>
+      <c r="H232" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>42513.641412037039</v>
+      </c>
+      <c r="B233" t="s">
+        <v>13</v>
+      </c>
+      <c r="C233">
+        <v>807858</v>
+      </c>
+      <c r="D233">
+        <v>3</v>
+      </c>
+      <c r="E233">
+        <v>10000</v>
+      </c>
+      <c r="F233" t="s">
+        <v>4</v>
+      </c>
+      <c r="G233">
+        <v>8</v>
+      </c>
+      <c r="H233" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>